<commit_message>
Dash: 85% + Doc
</commit_message>
<xml_diff>
--- a/Cronograma de Actividades.xlsx
+++ b/Cronograma de Actividades.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\2021-II\PROGRAMACION PARA ANALITICA DE DATOS\Competencias\Proyecto\ProyectosCarst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00CD5CF0-4910-49D2-B51F-54BEAEAC58AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C423A6EE-D2A7-4EB3-B749-E705B1AD05D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -340,7 +340,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -372,6 +372,39 @@
     </xf>
     <xf numFmtId="4" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -419,38 +452,14 @@
     <xf numFmtId="4" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -673,7 +682,7 @@
   <dimension ref="A1:AA1006"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -727,13 +736,13 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="30"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="17"/>
     </row>
     <row r="3" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="10">
@@ -755,7 +764,7 @@
       </c>
     </row>
     <row r="4" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="14">
+      <c r="A4" s="25">
         <v>2</v>
       </c>
       <c r="B4" s="10" t="s">
@@ -774,7 +783,7 @@
       </c>
     </row>
     <row r="5" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="14"/>
+      <c r="A5" s="25"/>
       <c r="B5" s="10" t="s">
         <v>20</v>
       </c>
@@ -791,7 +800,7 @@
       </c>
     </row>
     <row r="6" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="14"/>
+      <c r="A6" s="25"/>
       <c r="B6" s="10" t="s">
         <v>21</v>
       </c>
@@ -808,13 +817,13 @@
       </c>
     </row>
     <row r="7" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="14"/>
-      <c r="B7" s="15" t="s">
+      <c r="A7" s="25"/>
+      <c r="B7" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="17"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="28"/>
     </row>
     <row r="8" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="10">
@@ -858,106 +867,112 @@
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
     </row>
     <row r="11" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="34">
+      <c r="A11" s="12">
         <v>1</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="34">
+      <c r="C11" s="12">
         <v>12.5</v>
       </c>
-      <c r="D11" s="34">
+      <c r="D11" s="12">
         <v>12.5</v>
       </c>
-      <c r="E11" s="35">
+      <c r="E11" s="13">
         <f>C11-D11</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="36">
+      <c r="A12" s="21">
         <v>2</v>
       </c>
-      <c r="B12" s="37" t="s">
+      <c r="B12" s="14" t="s">
         <v>18</v>
       </c>
       <c r="C12" s="8">
         <v>6.25</v>
       </c>
       <c r="D12" s="8">
-        <v>3.25</v>
+        <v>5</v>
       </c>
       <c r="E12" s="9">
         <f>C12-D12</f>
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="22"/>
+      <c r="B13" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="12">
+        <v>6.25</v>
+      </c>
+      <c r="D13" s="12">
+        <v>6.25</v>
+      </c>
+      <c r="E13" s="13">
+        <f t="shared" ref="E13:E17" si="2">C13-D13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A14" s="21">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="38"/>
-      <c r="B13" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="8">
-        <v>6.25</v>
-      </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="9">
-        <f t="shared" ref="E13:E17" si="2">C13-D13</f>
-        <v>6.25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="31">
-        <v>3</v>
-      </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="41">
         <v>4.166666666666667</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4">
+      <c r="D14" s="41"/>
+      <c r="E14" s="41">
         <f t="shared" si="2"/>
         <v>4.166666666666667</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="32"/>
-      <c r="B15" s="6" t="s">
+      <c r="A15" s="39"/>
+      <c r="B15" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="13">
         <v>4.166666666666667</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4">
+      <c r="D15" s="13">
+        <v>4.17</v>
+      </c>
+      <c r="E15" s="13">
         <f t="shared" si="2"/>
+        <v>-3.3333333333329662E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A16" s="22"/>
+      <c r="B16" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="13">
         <v>4.166666666666667</v>
       </c>
-    </row>
-    <row r="16" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="33"/>
-      <c r="B16" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="4">
-        <v>4.166666666666667</v>
-      </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4">
+      <c r="D16" s="13">
+        <v>4.17</v>
+      </c>
+      <c r="E16" s="13">
         <f t="shared" si="2"/>
-        <v>4.166666666666667</v>
+        <v>-3.3333333333329662E-3</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
@@ -977,29 +992,29 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="19"/>
-      <c r="C18" s="22">
+      <c r="B18" s="30"/>
+      <c r="C18" s="33">
         <f>SUM(C3:C6)+SUM(C11:C17)+SUM(C8:C9)</f>
         <v>100</v>
       </c>
-      <c r="D18" s="24">
+      <c r="D18" s="35">
         <f>SUM(D3:D9,D11:D17)</f>
-        <v>65.75</v>
-      </c>
-      <c r="E18" s="26">
+        <v>82.09</v>
+      </c>
+      <c r="E18" s="37">
         <f>SUM(E11:E17)+SUM(E3:E6)+SUM(E8:E9)</f>
-        <v>34.25</v>
+        <v>17.91</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="20"/>
-      <c r="B19" s="21"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="27"/>
+      <c r="A19" s="31"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="38"/>
     </row>
     <row r="20" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
@@ -3966,16 +3981,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A14:A16"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A10:E10"/>
     <mergeCell ref="A4:A7"/>
     <mergeCell ref="B7:E7"/>
-    <mergeCell ref="A18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4015,13 +4030,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="30"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="17"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="10">
@@ -4040,7 +4055,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="14">
+      <c r="A4" s="25">
         <v>2</v>
       </c>
       <c r="B4" s="10" t="s">
@@ -4056,7 +4071,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="14"/>
+      <c r="A5" s="25"/>
       <c r="B5" s="10" t="s">
         <v>20</v>
       </c>
@@ -4070,7 +4085,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="14"/>
+      <c r="A6" s="25"/>
       <c r="B6" s="10" t="s">
         <v>21</v>
       </c>
@@ -4084,13 +4099,13 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="14"/>
-      <c r="B7" s="15" t="s">
+      <c r="A7" s="25"/>
+      <c r="B7" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="17"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="28"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="10">
@@ -4125,35 +4140,35 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="34">
+      <c r="A11" s="12">
         <v>1</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="34">
+      <c r="C11" s="12">
         <v>12.5</v>
       </c>
-      <c r="D11" s="34"/>
-      <c r="E11" s="35">
+      <c r="D11" s="12"/>
+      <c r="E11" s="13">
         <f>C11-D11</f>
         <v>12.5</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="36">
+      <c r="A12" s="21">
         <v>2</v>
       </c>
-      <c r="B12" s="37" t="s">
+      <c r="B12" s="14" t="s">
         <v>18</v>
       </c>
       <c r="C12" s="8">
@@ -4166,8 +4181,8 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="38"/>
-      <c r="B13" s="37" t="s">
+      <c r="A13" s="22"/>
+      <c r="B13" s="14" t="s">
         <v>19</v>
       </c>
       <c r="C13" s="8">
@@ -4180,7 +4195,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="31">
+      <c r="A14" s="18">
         <v>3</v>
       </c>
       <c r="B14" s="6" t="s">
@@ -4196,7 +4211,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="32"/>
+      <c r="A15" s="19"/>
       <c r="B15" s="6" t="s">
         <v>11</v>
       </c>
@@ -4210,7 +4225,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="33"/>
+      <c r="A16" s="20"/>
       <c r="B16" s="6" t="s">
         <v>12</v>
       </c>
@@ -4240,29 +4255,29 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="19"/>
-      <c r="C18" s="22">
+      <c r="B18" s="30"/>
+      <c r="C18" s="33">
         <f>SUM(C3:C6)+SUM(C11:C17)+SUM(C8:C9)</f>
         <v>100</v>
       </c>
-      <c r="D18" s="24">
+      <c r="D18" s="35">
         <f>SUM(D3:D9,D11:D17)</f>
         <v>0</v>
       </c>
-      <c r="E18" s="26">
+      <c r="E18" s="37">
         <f>SUM(E11:E17)+SUM(E3:E6)+SUM(E8:E9)</f>
         <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="20"/>
-      <c r="B19" s="21"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="27"/>
+      <c r="A19" s="31"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>